<commit_message>
[FCT] Add new features for planning optimisation
</commit_message>
<xml_diff>
--- a/EDT_EAH/bin/Debug/EDT_EAH.xlsx
+++ b/EDT_EAH/bin/Debug/EDT_EAH.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Perso\edt-eah\EDT_EAH\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\edt-eah\EDT_EAH\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F01C11D-4FC1-46EA-8ECF-976064DE53E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{AB4BD8E3-11D0-4585-9DB2-1CC211EA48BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="4" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="TeacherPlanning" sheetId="3" r:id="rId4"/>
     <sheet name="Planning" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="122">
   <si>
     <t>Code</t>
   </si>
@@ -49,28 +48,10 @@
     <t>Nom</t>
   </si>
   <si>
-    <t>Matière1</t>
-  </si>
-  <si>
-    <t>Matière2</t>
-  </si>
-  <si>
-    <t>Matière3</t>
-  </si>
-  <si>
     <t>SVT_L</t>
   </si>
   <si>
     <t>SVT_C</t>
-  </si>
-  <si>
-    <t>Matière4</t>
-  </si>
-  <si>
-    <t>Matière5</t>
-  </si>
-  <si>
-    <t>Matière6</t>
   </si>
   <si>
     <t>Version</t>
@@ -352,31 +333,13 @@
     <t>Hour</t>
   </si>
   <si>
-    <t>HDJ1</t>
-  </si>
-  <si>
-    <t>HDJ2</t>
-  </si>
-  <si>
-    <t>HDJ3</t>
-  </si>
-  <si>
     <t>11h00</t>
   </si>
   <si>
     <t>Carmen</t>
   </si>
   <si>
-    <t>Oumou</t>
-  </si>
-  <si>
     <t>PAUSE_DEJ</t>
-  </si>
-  <si>
-    <t>Maimouna</t>
-  </si>
-  <si>
-    <t>Shana</t>
   </si>
   <si>
     <t>Maxence</t>
@@ -388,28 +351,55 @@
     <t>Ninon</t>
   </si>
   <si>
-    <t>Messan</t>
-  </si>
-  <si>
-    <t>Mellissandre</t>
-  </si>
-  <si>
-    <t>Tiago</t>
-  </si>
-  <si>
-    <t>Yaelle</t>
-  </si>
-  <si>
     <t>Suzon</t>
   </si>
   <si>
-    <t xml:space="preserve">Céline </t>
+    <t>Maïmouna</t>
+  </si>
+  <si>
+    <t>Céline DUBOURDIEU</t>
+  </si>
+  <si>
+    <t>Matière 1</t>
+  </si>
+  <si>
+    <t>Matière 2</t>
+  </si>
+  <si>
+    <t>Matière 3</t>
+  </si>
+  <si>
+    <t>Matière 4</t>
+  </si>
+  <si>
+    <t>Matière 5</t>
+  </si>
+  <si>
+    <t>Matière 6</t>
+  </si>
+  <si>
+    <t>HDJ 1</t>
+  </si>
+  <si>
+    <t>Ethan</t>
+  </si>
+  <si>
+    <t>Mégane</t>
+  </si>
+  <si>
+    <t>Nasreddine</t>
+  </si>
+  <si>
+    <t>Jason</t>
+  </si>
+  <si>
+    <t>Claude ARDITTY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-40C]dddd\ d\ mmmm\ yyyy"/>
   </numFmts>
@@ -739,7 +729,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -854,6 +844,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -872,7 +871,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1167,33 +1166,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15E6115B-F90C-4E2F-ACB4-6651C02A7F36}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="9">
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1202,316 +1201,316 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04331DE5-6CED-468F-9298-889A169362F2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="67.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.81640625" customWidth="1"/>
+    <col min="2" max="2" width="67.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>37</v>
+      <c r="B14" s="16" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>37</v>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>37</v>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>42</v>
+      <c r="B25" s="14" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="15"/>
       <c r="B26" s="16"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="13"/>
       <c r="B27" s="14"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="15"/>
       <c r="B28" s="16"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
       <c r="B29" s="14"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="15"/>
       <c r="B30" s="16"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="13"/>
       <c r="B31" s="14"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="15"/>
       <c r="B32" s="16"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="13"/>
       <c r="B33" s="14"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="15"/>
       <c r="B34" s="16"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
       <c r="B35" s="14"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="15"/>
       <c r="B36" s="16"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="13"/>
       <c r="B37" s="14"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="15"/>
       <c r="B38" s="16"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="13"/>
       <c r="B39" s="14"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="15"/>
       <c r="B40" s="16"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="13"/>
       <c r="B41" s="14"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="15"/>
       <c r="B42" s="16"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="13"/>
       <c r="B43" s="14"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="15"/>
       <c r="B44" s="16"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="13"/>
       <c r="B45" s="14"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="15"/>
       <c r="B46" s="16"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="13"/>
       <c r="B47" s="14"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="15"/>
       <c r="B48" s="16"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="13"/>
       <c r="B49" s="14"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="17"/>
       <c r="B50" s="1"/>
     </row>
@@ -1522,48 +1521,48 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE1435D-036C-4820-AB48-1FB5DE56252A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" customWidth="1"/>
-    <col min="2" max="7" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" width="31.26953125" customWidth="1"/>
+    <col min="2" max="7" width="30.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>8</v>
+        <v>112</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>11</v>
+        <v>113</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>12</v>
+        <v>114</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -1571,9 +1570,9 @@
       <c r="F2" s="11"/>
       <c r="G2" s="12"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>4</v>
@@ -1584,42 +1583,42 @@
       <c r="F3" s="13"/>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
@@ -1627,9 +1626,9 @@
       <c r="F6" s="15"/>
       <c r="G6" s="16"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>3</v>
@@ -1642,15 +1641,15 @@
       <c r="F7" s="13"/>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>3</v>
@@ -1661,29 +1660,26 @@
       <c r="F8" s="15"/>
       <c r="G8" s="16"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="15"/>
@@ -1691,24 +1687,22 @@
       <c r="F10" s="15"/>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>4</v>
-      </c>
+      <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>4</v>
@@ -1719,12 +1713,12 @@
       <c r="F12" s="15"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -1732,9 +1726,9 @@
       <c r="F13" s="13"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>2</v>
@@ -1743,17 +1737,17 @@
         <v>1</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>3</v>
@@ -1766,12 +1760,12 @@
       <c r="F15" s="13"/>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -1779,12 +1773,12 @@
       <c r="F16" s="15"/>
       <c r="G16" s="16"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
@@ -1792,12 +1786,12 @@
       <c r="F17" s="13"/>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -1805,25 +1799,37 @@
       <c r="F18" s="15"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="16"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
@@ -1832,7 +1838,7 @@
       <c r="F21" s="13"/>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="15"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -1841,7 +1847,7 @@
       <c r="F22" s="15"/>
       <c r="G22" s="16"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -1850,7 +1856,7 @@
       <c r="F23" s="13"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -1859,7 +1865,7 @@
       <c r="F24" s="15"/>
       <c r="G24" s="16"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -1868,7 +1874,7 @@
       <c r="F25" s="13"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -1877,7 +1883,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="16"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
@@ -1886,7 +1892,7 @@
       <c r="F27" s="13"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="15"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -1895,7 +1901,7 @@
       <c r="F28" s="15"/>
       <c r="G28" s="16"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -1904,7 +1910,7 @@
       <c r="F29" s="13"/>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="15"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -1913,7 +1919,7 @@
       <c r="F30" s="15"/>
       <c r="G30" s="16"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -1922,7 +1928,7 @@
       <c r="F31" s="13"/>
       <c r="G31" s="14"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="15"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -1931,7 +1937,7 @@
       <c r="F32" s="15"/>
       <c r="G32" s="16"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -1940,7 +1946,7 @@
       <c r="F33" s="13"/>
       <c r="G33" s="14"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="15"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -1949,7 +1955,7 @@
       <c r="F34" s="15"/>
       <c r="G34" s="16"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -1958,7 +1964,7 @@
       <c r="F35" s="13"/>
       <c r="G35" s="14"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="17"/>
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
@@ -1970,14 +1976,15 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9B7CE21E-B116-44A6-B472-28200735DC58}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>FieldAreas!$A$2:$A$50</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:G36</xm:sqref>
+          <xm:sqref>B2:G9 B11:G36 D10:G10 B10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1986,41 +1993,43 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E6308A-C377-41B7-86DE-13B86820C00B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23:U28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15.26953125" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" style="32" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="32" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" style="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" style="32" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" style="32" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="32" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" style="32" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.140625" style="32" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" style="32" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.26953125" style="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7265625" style="32" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.453125" style="32" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.1796875" style="32" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.1796875" style="32" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7265625" style="32" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16" style="32" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" style="32" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.54296875" style="32" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.7265625" style="32" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18" style="32" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" style="32" bestFit="1" customWidth="1"/>
-    <col min="20" max="37" width="8.140625" customWidth="1"/>
+    <col min="19" max="19" width="14.1796875" style="32" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.54296875" customWidth="1"/>
+    <col min="21" max="21" width="22.26953125" customWidth="1"/>
+    <col min="22" max="37" width="8.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="45" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C1" s="46" t="str">
         <f>Teachers!A2</f>
@@ -2090,12 +2099,13 @@
         <f>Teachers!A18</f>
         <v>Alain RENAUD</v>
       </c>
-      <c r="T1" s="45" t="s">
-        <v>124</v>
-      </c>
-      <c r="U1" s="45">
+      <c r="T1" s="45" t="str">
+        <f>Teachers!A19</f>
+        <v>Céline DUBOURDIEU</v>
+      </c>
+      <c r="U1" s="45" t="str">
         <f>Teachers!A20</f>
-        <v>0</v>
+        <v>Claude ARDITTY</v>
       </c>
       <c r="V1" s="45">
         <f>Teachers!A21</f>
@@ -2162,18 +2172,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" s="33" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E2" s="35"/>
       <c r="F2" s="35"/>
@@ -2209,19 +2219,19 @@
       <c r="AJ2" s="34"/>
       <c r="AK2" s="36"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" s="37"/>
       <c r="B3" s="13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F3" s="31"/>
       <c r="G3" s="31"/>
@@ -2256,19 +2266,19 @@
       <c r="AJ3" s="13"/>
       <c r="AK3" s="38"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4" s="39"/>
       <c r="B4" s="15" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
@@ -2303,16 +2313,16 @@
       <c r="AJ4" s="15"/>
       <c r="AK4" s="40"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5" s="37"/>
       <c r="B5" s="13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E5" s="31"/>
       <c r="F5" s="31"/>
@@ -2348,10 +2358,10 @@
       <c r="AJ5" s="13"/>
       <c r="AK5" s="38"/>
     </row>
-    <row r="6" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="53"/>
       <c r="B6" s="51" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C6" s="54"/>
       <c r="D6" s="54"/>
@@ -2389,10 +2399,10 @@
       <c r="AJ6" s="51"/>
       <c r="AK6" s="55"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A7" s="39"/>
       <c r="B7" s="15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C7" s="30"/>
       <c r="D7" s="30"/>
@@ -2430,10 +2440,10 @@
       <c r="AJ7" s="15"/>
       <c r="AK7" s="40"/>
     </row>
-    <row r="8" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="41"/>
       <c r="B8" s="42" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C8" s="43"/>
       <c r="D8" s="43"/>
@@ -2471,21 +2481,21 @@
       <c r="AJ8" s="42"/>
       <c r="AK8" s="44"/>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A9" s="33" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D9" s="35"/>
       <c r="E9" s="35"/>
       <c r="F9" s="35"/>
       <c r="G9" s="35" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="H9" s="35"/>
       <c r="I9" s="35"/>
@@ -2518,24 +2528,24 @@
       <c r="AJ9" s="34"/>
       <c r="AK9" s="36"/>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A10" s="37"/>
       <c r="B10" s="13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D10" s="31"/>
       <c r="E10" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F10" s="31"/>
       <c r="G10" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="H10" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I10" s="31"/>
       <c r="J10" s="31"/>
@@ -2567,24 +2577,24 @@
       <c r="AJ10" s="13"/>
       <c r="AK10" s="38"/>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A11" s="39"/>
       <c r="B11" s="15" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D11" s="30"/>
       <c r="E11" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F11" s="30"/>
       <c r="G11" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="H11" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I11" s="30"/>
       <c r="J11" s="30"/>
@@ -2616,24 +2626,24 @@
       <c r="AJ11" s="15"/>
       <c r="AK11" s="40"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A12" s="37"/>
       <c r="B12" s="13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D12" s="31"/>
       <c r="E12" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F12" s="31"/>
       <c r="G12" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="H12" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I12" s="31"/>
       <c r="J12" s="31"/>
@@ -2665,10 +2675,10 @@
       <c r="AJ12" s="13"/>
       <c r="AK12" s="38"/>
     </row>
-    <row r="13" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="53"/>
       <c r="B13" s="51" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C13" s="54"/>
       <c r="D13" s="54"/>
@@ -2706,10 +2716,10 @@
       <c r="AJ13" s="51"/>
       <c r="AK13" s="55"/>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A14" s="39"/>
       <c r="B14" s="15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C14" s="30"/>
       <c r="D14" s="30"/>
@@ -2747,10 +2757,10 @@
       <c r="AJ14" s="15"/>
       <c r="AK14" s="40"/>
     </row>
-    <row r="15" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="41"/>
       <c r="B15" s="42" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="43"/>
@@ -2788,12 +2798,12 @@
       <c r="AJ15" s="42"/>
       <c r="AK15" s="44"/>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A16" s="33" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C16" s="35"/>
       <c r="D16" s="35"/>
@@ -2831,10 +2841,10 @@
       <c r="AJ16" s="34"/>
       <c r="AK16" s="36"/>
     </row>
-    <row r="17" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A17" s="37"/>
       <c r="B17" s="13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="31"/>
@@ -2872,10 +2882,10 @@
       <c r="AJ17" s="13"/>
       <c r="AK17" s="38"/>
     </row>
-    <row r="18" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A18" s="39"/>
       <c r="B18" s="15" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
@@ -2913,10 +2923,10 @@
       <c r="AJ18" s="15"/>
       <c r="AK18" s="40"/>
     </row>
-    <row r="19" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A19" s="37"/>
       <c r="B19" s="13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="31"/>
@@ -2954,10 +2964,10 @@
       <c r="AJ19" s="13"/>
       <c r="AK19" s="38"/>
     </row>
-    <row r="20" spans="1:16384" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16384" s="52" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="51"/>
       <c r="B20" s="51" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C20" s="51"/>
       <c r="D20" s="51"/>
@@ -19342,10 +19352,10 @@
       <c r="XFC20" s="51"/>
       <c r="XFD20" s="51"/>
     </row>
-    <row r="21" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A21" s="39"/>
       <c r="B21" s="15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
@@ -19383,10 +19393,10 @@
       <c r="AJ21" s="15"/>
       <c r="AK21" s="40"/>
     </row>
-    <row r="22" spans="1:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16384" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="41"/>
       <c r="B22" s="42" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C22" s="43"/>
       <c r="D22" s="43"/>
@@ -19424,12 +19434,12 @@
       <c r="AJ22" s="42"/>
       <c r="AK22" s="44"/>
     </row>
-    <row r="23" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A23" s="33" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C23" s="35"/>
       <c r="D23" s="35"/>
@@ -19439,21 +19449,21 @@
       <c r="H23" s="35"/>
       <c r="I23" s="35"/>
       <c r="J23" s="35" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="K23" s="35"/>
       <c r="L23" s="35"/>
       <c r="M23" s="35"/>
       <c r="N23" s="35"/>
-      <c r="O23" s="35" t="s">
-        <v>89</v>
-      </c>
+      <c r="O23" s="35"/>
       <c r="P23" s="35"/>
       <c r="Q23" s="35"/>
       <c r="R23" s="35"/>
       <c r="S23" s="35"/>
       <c r="T23" s="34"/>
-      <c r="U23" s="34"/>
+      <c r="U23" s="60" t="s">
+        <v>83</v>
+      </c>
       <c r="V23" s="34"/>
       <c r="W23" s="34"/>
       <c r="X23" s="34"/>
@@ -19471,10 +19481,10 @@
       <c r="AJ23" s="34"/>
       <c r="AK23" s="36"/>
     </row>
-    <row r="24" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A24" s="37"/>
       <c r="B24" s="13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C24" s="31"/>
       <c r="D24" s="31"/>
@@ -19484,29 +19494,29 @@
       <c r="H24" s="31"/>
       <c r="I24" s="31"/>
       <c r="J24" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="K24" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="L24" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="M24" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="N24" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="O24" s="31" t="s">
-        <v>89</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="O24" s="31"/>
       <c r="P24" s="31"/>
       <c r="Q24" s="31"/>
       <c r="R24" s="31"/>
       <c r="S24" s="31"/>
       <c r="T24" s="13"/>
-      <c r="U24" s="13"/>
+      <c r="U24" s="61" t="s">
+        <v>83</v>
+      </c>
       <c r="V24" s="13"/>
       <c r="W24" s="13"/>
       <c r="X24" s="13"/>
@@ -19524,10 +19534,10 @@
       <c r="AJ24" s="13"/>
       <c r="AK24" s="38"/>
     </row>
-    <row r="25" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A25" s="39"/>
       <c r="B25" s="15" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
@@ -19537,29 +19547,29 @@
       <c r="H25" s="30"/>
       <c r="I25" s="30"/>
       <c r="J25" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="K25" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="L25" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="M25" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="N25" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="O25" s="30" t="s">
-        <v>89</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="O25" s="30"/>
       <c r="P25" s="30"/>
       <c r="Q25" s="30"/>
       <c r="R25" s="30"/>
       <c r="S25" s="30"/>
       <c r="T25" s="15"/>
-      <c r="U25" s="15"/>
+      <c r="U25" s="62" t="s">
+        <v>83</v>
+      </c>
       <c r="V25" s="15"/>
       <c r="W25" s="15"/>
       <c r="X25" s="15"/>
@@ -19577,10 +19587,10 @@
       <c r="AJ25" s="15"/>
       <c r="AK25" s="40"/>
     </row>
-    <row r="26" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A26" s="37"/>
       <c r="B26" s="13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C26" s="31"/>
       <c r="D26" s="31"/>
@@ -19589,30 +19599,28 @@
       <c r="G26" s="31"/>
       <c r="H26" s="31"/>
       <c r="I26" s="31"/>
-      <c r="J26" s="31" t="s">
-        <v>89</v>
-      </c>
+      <c r="J26" s="31"/>
       <c r="K26" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="L26" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="M26" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="N26" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="O26" s="31" t="s">
-        <v>89</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="O26" s="31"/>
       <c r="P26" s="31"/>
       <c r="Q26" s="31"/>
       <c r="R26" s="31"/>
       <c r="S26" s="31"/>
       <c r="T26" s="13"/>
-      <c r="U26" s="13"/>
+      <c r="U26" s="61" t="s">
+        <v>83</v>
+      </c>
       <c r="V26" s="13"/>
       <c r="W26" s="13"/>
       <c r="X26" s="13"/>
@@ -19630,10 +19638,10 @@
       <c r="AJ26" s="13"/>
       <c r="AK26" s="38"/>
     </row>
-    <row r="27" spans="1:16384" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16384" s="52" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="53"/>
       <c r="B27" s="51" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C27" s="54"/>
       <c r="D27" s="54"/>
@@ -19671,10 +19679,10 @@
       <c r="AJ27" s="51"/>
       <c r="AK27" s="55"/>
     </row>
-    <row r="28" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A28" s="39"/>
       <c r="B28" s="15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C28" s="30"/>
       <c r="D28" s="30"/>
@@ -19685,16 +19693,16 @@
       <c r="I28" s="30"/>
       <c r="J28" s="30"/>
       <c r="K28" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="L28" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="M28" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="N28" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="O28" s="30"/>
       <c r="P28" s="30"/>
@@ -19720,10 +19728,10 @@
       <c r="AJ28" s="15"/>
       <c r="AK28" s="40"/>
     </row>
-    <row r="29" spans="1:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16384" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="41"/>
       <c r="B29" s="42" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C29" s="43"/>
       <c r="D29" s="43"/>
@@ -19734,16 +19742,16 @@
       <c r="I29" s="43"/>
       <c r="J29" s="43"/>
       <c r="K29" s="43" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="L29" s="43" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="M29" s="43" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="N29" s="43" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="O29" s="43"/>
       <c r="P29" s="43"/>
@@ -19769,12 +19777,12 @@
       <c r="AJ29" s="42"/>
       <c r="AK29" s="44"/>
     </row>
-    <row r="30" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A30" s="33" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C30" s="35"/>
       <c r="D30" s="35"/>
@@ -19788,12 +19796,14 @@
       <c r="L30" s="35"/>
       <c r="M30" s="35"/>
       <c r="N30" s="35"/>
-      <c r="O30" s="35"/>
+      <c r="O30" s="35" t="s">
+        <v>83</v>
+      </c>
       <c r="P30" s="35" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="Q30" s="35" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R30" s="35"/>
       <c r="S30" s="35"/>
@@ -19816,10 +19826,10 @@
       <c r="AJ30" s="34"/>
       <c r="AK30" s="36"/>
     </row>
-    <row r="31" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A31" s="37"/>
       <c r="B31" s="13" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C31" s="31"/>
       <c r="D31" s="31"/>
@@ -19833,15 +19843,19 @@
       <c r="L31" s="31"/>
       <c r="M31" s="31"/>
       <c r="N31" s="31"/>
-      <c r="O31" s="31"/>
+      <c r="O31" s="31" t="s">
+        <v>83</v>
+      </c>
       <c r="P31" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="Q31" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R31" s="31"/>
-      <c r="S31" s="31"/>
+      <c r="S31" s="31" t="s">
+        <v>83</v>
+      </c>
       <c r="T31" s="13"/>
       <c r="U31" s="13"/>
       <c r="V31" s="13"/>
@@ -19861,10 +19875,10 @@
       <c r="AJ31" s="13"/>
       <c r="AK31" s="38"/>
     </row>
-    <row r="32" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A32" s="39"/>
       <c r="B32" s="15" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C32" s="30"/>
       <c r="D32" s="30"/>
@@ -19878,12 +19892,14 @@
       <c r="L32" s="30"/>
       <c r="M32" s="30"/>
       <c r="N32" s="30"/>
-      <c r="O32" s="30"/>
+      <c r="O32" s="30" t="s">
+        <v>83</v>
+      </c>
       <c r="P32" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="Q32" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R32" s="30"/>
       <c r="S32" s="30"/>
@@ -19906,10 +19922,10 @@
       <c r="AJ32" s="15"/>
       <c r="AK32" s="40"/>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A33" s="37"/>
       <c r="B33" s="13" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C33" s="31"/>
       <c r="D33" s="31"/>
@@ -19923,12 +19939,14 @@
       <c r="L33" s="31"/>
       <c r="M33" s="31"/>
       <c r="N33" s="31"/>
-      <c r="O33" s="31"/>
+      <c r="O33" s="31" t="s">
+        <v>83</v>
+      </c>
       <c r="P33" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="Q33" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R33" s="31"/>
       <c r="S33" s="31"/>
@@ -19951,10 +19969,10 @@
       <c r="AJ33" s="13"/>
       <c r="AK33" s="38"/>
     </row>
-    <row r="34" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="53"/>
       <c r="B34" s="51" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C34" s="54"/>
       <c r="D34" s="54"/>
@@ -19992,10 +20010,10 @@
       <c r="AJ34" s="51"/>
       <c r="AK34" s="55"/>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A35" s="39"/>
       <c r="B35" s="15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C35" s="30"/>
       <c r="D35" s="30"/>
@@ -20033,10 +20051,10 @@
       <c r="AJ35" s="15"/>
       <c r="AK35" s="40"/>
     </row>
-    <row r="36" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="41"/>
       <c r="B36" s="42" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C36" s="43"/>
       <c r="D36" s="43"/>
@@ -20081,116 +20099,120 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B354B981-67DC-47C1-9057-005B7C036602}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="3" customWidth="1"/>
-    <col min="4" max="9" width="18.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="18.26953125" style="3" customWidth="1"/>
+    <col min="4" max="9" width="18.453125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C1" s="4">
-        <v>44102</v>
+        <v>44105</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="47" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>8</v>
+        <v>112</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>11</v>
+        <v>113</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>12</v>
+        <v>114</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I2" s="20"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="22"/>
+      <c r="D3" s="62" t="s">
+        <v>1</v>
+      </c>
       <c r="E3" s="22"/>
       <c r="F3" s="22"/>
       <c r="G3" s="22"/>
       <c r="H3" s="22"/>
       <c r="I3" s="23"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="48" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="C4" s="25"/>
+        <v>107</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>3</v>
+      </c>
       <c r="D4" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="25"/>
+        <v>1</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>37</v>
+      </c>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
       <c r="I4" s="26"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="22"/>
+        <v>3</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>2</v>
+      </c>
       <c r="E5" s="22"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
       <c r="I5" s="23"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>4</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="25"/>
       <c r="D6" s="25"/>
       <c r="E6" s="25"/>
       <c r="F6" s="25"/>
@@ -20198,122 +20220,154 @@
       <c r="H6" s="25"/>
       <c r="I6" s="26"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="22"/>
+        <v>104</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>1</v>
+      </c>
       <c r="D7" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="22"/>
+        <v>4</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>37</v>
+      </c>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
       <c r="I7" s="23"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="48" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
+        <v>105</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="E8" s="25"/>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
       <c r="I8" s="26"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
+        <v>90</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>2</v>
+      </c>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
       <c r="I9" s="23"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="48" t="s">
-        <v>97</v>
-      </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
+        <v>91</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>1</v>
+      </c>
       <c r="E10" s="25"/>
       <c r="F10" s="25"/>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
       <c r="I10" s="26"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
+        <v>3</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>37</v>
+      </c>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
       <c r="I11" s="23"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="48" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
+        <v>3</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>2</v>
+      </c>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="26"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="22"/>
+        <v>37</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>1</v>
+      </c>
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
       <c r="I13" s="23"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="48" t="s">
-        <v>101</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>119</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="B14" s="24"/>
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
@@ -20322,9 +20376,9 @@
       <c r="H14" s="25"/>
       <c r="I14" s="26"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>120</v>
@@ -20332,22 +20386,16 @@
       <c r="C15" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="22" t="s">
-        <v>61</v>
-      </c>
+      <c r="D15" s="22"/>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
       <c r="G15" s="22"/>
       <c r="H15" s="22"/>
       <c r="I15" s="23"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="48" t="s">
-        <v>108</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>121</v>
-      </c>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="48"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
       <c r="E16" s="25"/>
@@ -20356,13 +20404,9 @@
       <c r="H16" s="25"/>
       <c r="I16" s="26"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B17" s="27" t="s">
-        <v>122</v>
-      </c>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="2"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -20371,13 +20415,13 @@
       <c r="H17" s="6"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="47" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B19" s="50" t="str">
         <f>UPPER(TEXT(C1,"jjjj"))</f>
-        <v>LUNDI</v>
+        <v>JEUDI</v>
       </c>
       <c r="C19" s="28" t="str">
         <f>IF($B$19="VENDREDI","9h15","9h30")</f>
@@ -20396,41 +20440,45 @@
         <v>11h45</v>
       </c>
       <c r="G19" s="56" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="H19" s="28" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="I19" s="29" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="str">
         <f>A3</f>
         <v>A</v>
       </c>
       <c r="B20" s="2" t="str">
         <f>B3</f>
-        <v>Oumou</v>
+        <v>Ethan</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G20" s="57"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="23"/>
+      <c r="H20" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="48" t="str">
         <f t="shared" ref="A21:B34" si="0">A4</f>
         <v>B</v>
@@ -20440,72 +20488,72 @@
         <v>Suzon</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G21" s="58"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="26"/>
+      <c r="H21" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="I21" s="26" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>C</v>
       </c>
       <c r="B22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Maimouna</v>
+        <v>Maïmouna</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G22" s="57"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="23"/>
+      <c r="H22" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="48" t="str">
         <f t="shared" si="0"/>
         <v>D</v>
       </c>
-      <c r="B23" s="48" t="str">
+      <c r="B23" s="48">
         <f t="shared" si="0"/>
-        <v>Shana</v>
-      </c>
-      <c r="C23" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="F23" s="25" t="s">
-        <v>89</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C23" s="48"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
       <c r="G23" s="58"/>
       <c r="H23" s="25"/>
       <c r="I23" s="26"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
@@ -20515,22 +20563,24 @@
         <v>Maxence</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G24" s="57"/>
-      <c r="H24" s="22"/>
+      <c r="H24" s="22" t="s">
+        <v>83</v>
+      </c>
       <c r="I24" s="23"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="48" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
@@ -20539,49 +20589,75 @@
         <f t="shared" si="0"/>
         <v>Salim</v>
       </c>
-      <c r="C25" s="48"/>
+      <c r="C25" s="48" t="s">
+        <v>83</v>
+      </c>
       <c r="D25" s="25"/>
       <c r="E25" s="25"/>
       <c r="F25" s="25"/>
       <c r="G25" s="58"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="26"/>
+      <c r="H25" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="I25" s="26" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>G</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
+        <v>Mégane</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>83</v>
+      </c>
       <c r="G26" s="57"/>
       <c r="H26" s="22"/>
       <c r="I26" s="23"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="48" t="str">
         <f t="shared" si="0"/>
         <v>H</v>
       </c>
-      <c r="B27" s="48">
+      <c r="B27" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C27" s="48"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
+        <v>Nasreddine</v>
+      </c>
+      <c r="C27" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>83</v>
+      </c>
       <c r="G27" s="58"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="26"/>
+      <c r="H27" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="I27" s="26" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -20590,23 +20666,27 @@
         <f t="shared" si="0"/>
         <v>Ninon</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>89</v>
+      <c r="C28" s="22" t="s">
+        <v>83</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F28" s="22" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G28" s="57"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="23"/>
+      <c r="H28" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="I28" s="23" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="48" t="str">
         <f t="shared" si="0"/>
         <v>J</v>
@@ -20616,22 +20696,26 @@
         <v>Carmen</v>
       </c>
       <c r="C29" s="48" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G29" s="58"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="26"/>
+      <c r="H29" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="I29" s="26" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="str">
         <f t="shared" si="0"/>
         <v>K</v>
@@ -20642,22 +20726,28 @@
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
+      <c r="E30" s="22" t="s">
+        <v>83</v>
+      </c>
       <c r="F30" s="22" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G30" s="57"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="23"/>
+      <c r="H30" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="I30" s="23" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="48" t="str">
         <f t="shared" si="0"/>
         <v>L</v>
       </c>
-      <c r="B31" s="48" t="str">
+      <c r="B31" s="48">
         <f t="shared" si="0"/>
-        <v>Messan</v>
+        <v>0</v>
       </c>
       <c r="C31" s="48"/>
       <c r="D31" s="25"/>
@@ -20667,35 +20757,35 @@
       <c r="H31" s="25"/>
       <c r="I31" s="26"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>HDJ1</v>
+        <f>A15</f>
+        <v>HDJ 1</v>
       </c>
       <c r="B32" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Mellissandre</v>
+        <v>Jason</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="22"/>
       <c r="E32" s="22" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G32" s="57"/>
       <c r="H32" s="22"/>
       <c r="I32" s="23"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="48" t="str">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="48">
         <f t="shared" si="0"/>
-        <v>HDJ2</v>
-      </c>
-      <c r="B33" s="48" t="str">
+        <v>0</v>
+      </c>
+      <c r="B33" s="48">
         <f t="shared" si="0"/>
-        <v>Tiago</v>
+        <v>0</v>
       </c>
       <c r="C33" s="48"/>
       <c r="D33" s="25"/>
@@ -20705,14 +20795,14 @@
       <c r="H33" s="25"/>
       <c r="I33" s="26"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="str">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
         <f t="shared" si="0"/>
-        <v>HDJ3</v>
-      </c>
-      <c r="B34" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="B34" s="2">
         <f t="shared" si="0"/>
-        <v>Yaelle</v>
+        <v>0</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="6"/>
@@ -20722,10 +20812,10 @@
       <c r="H34" s="6"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C35" s="49"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C36"/>
     </row>
   </sheetData>
@@ -20734,7 +20824,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{30B4E95C-DF9F-4CEA-B9CC-05128F1311B3}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>FieldAreas!$A$2:$A$50</xm:f>
           </x14:formula1>

</xml_diff>